<commit_message>
2023-08-13 update cosmetic backlog
</commit_message>
<xml_diff>
--- a/public/dunbin_backlog.xlsx
+++ b/public/dunbin_backlog.xlsx
@@ -1732,7 +1732,7 @@
         <v>updated</v>
       </c>
       <c r="C16" t="str">
-        <v>s</v>
+        <v/>
       </c>
       <c r="D16" t="str">
         <v/>
@@ -1786,16 +1786,16 @@
         <v/>
       </c>
       <c r="U16" t="str">
-        <v>s</v>
+        <v/>
       </c>
       <c r="V16" t="str">
         <v/>
       </c>
-      <c r="W16">
-        <v>1</v>
-      </c>
-      <c r="X16">
-        <v>1</v>
+      <c r="W16" t="str">
+        <v/>
+      </c>
+      <c r="X16" t="str">
+        <v/>
       </c>
       <c r="Y16" t="str">
         <v/>

</xml_diff>